<commit_message>
2/9/25 falta solo postergar semanas y tropas
</commit_message>
<xml_diff>
--- a/pruebas y controles.xlsx
+++ b/pruebas y controles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="78">
   <si>
     <t>COD</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>orden</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -833,8 +836,8 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2133,10 +2136,18 @@
       <c r="E47" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="12"/>
+      <c r="F47" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="H47" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="I47" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J47" s="13"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -2177,10 +2188,18 @@
       <c r="E49" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="12"/>
+      <c r="F49" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="H49" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="I49" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J49" s="13" t="s">
         <v>9</v>
       </c>
@@ -2225,16 +2244,18 @@
       <c r="E51" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I51" s="12"/>
+      <c r="F51" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H51" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I51" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J51" s="13"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
@@ -2253,16 +2274,18 @@
       <c r="E52" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F52" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I52" s="12"/>
+      <c r="F52" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H52" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I52" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
@@ -2279,10 +2302,18 @@
       <c r="E53" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="12"/>
+      <c r="F53" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G53" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H53" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I53" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
@@ -2299,10 +2330,18 @@
       <c r="E54" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="12"/>
+      <c r="F54" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H54" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I54" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
@@ -2319,10 +2358,18 @@
       <c r="E55" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="I55" s="12"/>
+      <c r="F55" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G55" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H55" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
@@ -2339,10 +2386,18 @@
       <c r="E56" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="12"/>
+      <c r="F56" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H56" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I56" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
@@ -2359,10 +2414,18 @@
       <c r="E57" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="12"/>
+      <c r="F57" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G57" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H57" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I57" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
@@ -2379,10 +2442,18 @@
       <c r="E58" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="12"/>
+      <c r="F58" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G58" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H58" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I58" s="34" t="s">
+        <v>75</v>
+      </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
@@ -2401,10 +2472,18 @@
       <c r="E59" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="12"/>
+      <c r="F59" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H59" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I59" s="34" t="s">
+        <v>77</v>
+      </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
@@ -2423,10 +2502,18 @@
       <c r="E60" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="12"/>
+      <c r="F60" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G60" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="H60" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I60" s="34" t="s">
+        <v>77</v>
+      </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>

</xml_diff>